<commit_message>
fix(import-sub-category): make import sub category into standalone component
</commit_message>
<xml_diff>
--- a/public/sub_category_data.xlsx
+++ b/public/sub_category_data.xlsx
@@ -397,42 +397,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>company_code</v>
+      </c>
+      <c r="B1" t="str">
+        <v>branch_code</v>
+      </c>
+      <c r="C1" t="str">
+        <v>category_code</v>
+      </c>
+      <c r="D1" t="str">
+        <v>code</v>
+      </c>
+      <c r="E1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
-        <v>category_name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>company_name</v>
-      </c>
-      <c r="D1" t="str">
-        <v>branch_name</v>
+      <c r="F1" t="str">
+        <v>description</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sub Cat</v>
+        <v>C001</v>
       </c>
       <c r="B2" t="str">
-        <v>Cat</v>
+        <v>B001</v>
       </c>
       <c r="C2" t="str">
-        <v>Company Name</v>
+        <v>CAT001</v>
       </c>
       <c r="D2" t="str">
-        <v>Head Office</v>
+        <v>SUBC001</v>
+      </c>
+      <c r="E2" t="str">
+        <v>sub category pertama</v>
+      </c>
+      <c r="F2" t="str">
+        <v>description  sub category pertama</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>C002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>B002</v>
+      </c>
+      <c r="C3" t="str">
+        <v>CAT002</v>
+      </c>
+      <c r="D3" t="str">
+        <v>SUBC002</v>
+      </c>
+      <c r="E3" t="str">
+        <v>sub categoroy kedua</v>
+      </c>
+      <c r="F3" t="str">
+        <v>description sub category kedua</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>